<commit_message>
Write field values using proper java reflection.
Using Field.set(obj, value) to write the actual values to the fields -
this reduces the overhead of checking for a setter method.
Also ensures that primitives can be written without fault.
Updated the LocalDateConverter class to handle exceptions aswell
</commit_message>
<xml_diff>
--- a/src/test/resources/test_people.xlsx
+++ b/src/test/resources/test_people.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikani\projects\labs\zerocell\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikani\projects\labs\zerocell\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Mpulula</t>
+  </si>
+  <si>
+    <t>FAV_NUMBER</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +419,7 @@
     <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +435,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,8 +455,11 @@
       <c r="E2" s="1">
         <v>34062</v>
       </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -463,8 +472,11 @@
       <c r="E3" s="1">
         <v>34475</v>
       </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -480,8 +492,11 @@
       <c r="E4" s="1">
         <v>32198</v>
       </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -497,8 +512,11 @@
       <c r="E5" s="1">
         <v>31507</v>
       </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -513,6 +531,9 @@
       </c>
       <c r="E6" s="1">
         <v>33613</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle incorrectly named/missing columns, add tests
Improved the code to handle incorrect or missing columns - for cases
where users try to upload a file with columns that are not defined on
in the annotations.
Added test cases for the various exceptions and their messages.
Finally, instances of ZeroCellException are just bubbled up instead of
being wrapped in another ZCE
</commit_message>
<xml_diff>
--- a/src/test/resources/test_people.xlsx
+++ b/src/test/resources/test_people.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikani\projects\labs\zerocell\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikani\projects\zerocell\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,12 +32,6 @@
     <t>FIRST_NAME</t>
   </si>
   <si>
-    <t>MIDDLENAME</t>
-  </si>
-  <si>
-    <t>LASTNAME</t>
-  </si>
-  <si>
     <t>DATE_OF_BIRTH</t>
   </si>
   <si>
@@ -87,6 +81,12 @@
   </si>
   <si>
     <t>DATE_REGISTERED</t>
+  </si>
+  <si>
+    <t>MIDDLE_NAME</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,19 +431,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -451,13 +451,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
         <v>34062</v>
@@ -474,10 +474,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
         <v>34475</v>
@@ -494,13 +494,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>32198</v>
@@ -517,13 +517,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>31507</v>
@@ -540,13 +540,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="1">
         <v>33613</v>

</xml_diff>